<commit_message>
Adicionada regra de combinação para solvatação
</commit_message>
<xml_diff>
--- a/Planilhas de análise/DADOS_PURO.xlsx
+++ b/Planilhas de análise/DADOS_PURO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="807" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="807" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Lista" sheetId="1" r:id="rId1"/>
@@ -1161,6 +1161,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>P x T</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2664,6 +2689,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>T (K)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2726,6 +2806,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>P (kPa)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6327,7 +6462,7 @@
   <dimension ref="B21:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6392,8 +6527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:G202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8131,8 +8266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:Q81"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8367,8 +8502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:Y51"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8554,8 +8689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ajustes nos comentários e fugacidade de SRK
</commit_message>
<xml_diff>
--- a/Planilhas de análise/DADOS_PURO.xlsx
+++ b/Planilhas de análise/DADOS_PURO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="807" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="807" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lista" sheetId="1" r:id="rId1"/>
@@ -1147,6 +1147,1251 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Etanol!$AA$3:$AA$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>197.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>203.88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>210.32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>216.76</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>223.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>229.64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>236.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>242.52</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>248.96</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>255.4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>261.83999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>268.27999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>274.72000000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>281.16000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>287.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>294.04000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>300.48</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>306.92</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>313.36</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>319.8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>326.24</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>332.68</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>339.12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>345.56</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>358.44</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>364.88</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>371.32</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>377.76</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>384.2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>390.64</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>397.08</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>403.52</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>409.96</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>416.4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>422.84</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>429.28</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>435.72</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>442.16</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>448.6</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>455.04</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>461.48</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>467.92</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>474.36</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>480.8</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>487.24</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>493.68</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>500.12</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>506.56</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>513</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Etanol!$AC$3:$AC$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>19170.521739130436</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19051.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18931.521739130436</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18810.565217391304</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18688.58695652174</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18565.58695652174</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18441.478260869564</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18316.260869565216</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18189.869565217392</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18062.26086956522</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17933.41304347826</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17803.217391304348</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17671.67391304348</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17538.717391304348</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17404.239130434784</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17268.217391304348</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17130.565217391304</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16991.217391304348</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16850.065217391304</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16707.021739130436</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16562</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16414.869565217392</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>16265.54347826087</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16113.891304347828</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>15959.739130434784</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>15802.956521739132</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15643.347826086958</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>15480.760869565218</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>15314.956521739132</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15145.695652173914</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14972.695652173914</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>14795.673913043478</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>14614.282608695652</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>14428.108695652174</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>14236.695652173914</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>14039.521739130434</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>13835.913043478262</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>13625.130434782608</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>13406.282608695652</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>13178.217391304348</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>12939.565217391306</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>12688.565217391304</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>12422.869565217392</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>12139.413043478262</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>11833.847826086956</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>11499.869565217392</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>11127.565217391304</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>10699.739130434782</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>10181.869565217392</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>9480.2608695652179</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>7709.652173913044</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B2BE-479E-9001-C8AEBD48EE04}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>CPA</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Etanol!$AD$3:$AD$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>302</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>314</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>322</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>326</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>332</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>342</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>346</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>348</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>354</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>356</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>358</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>362</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>364</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>368</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>372</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>374</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>376</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>378</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>382</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>386</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>388</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>392</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>394</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>396</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>398</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>402</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>404</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>406</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>408</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>422</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>428</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>434</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>438</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>442</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>444</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>446</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>452</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>454</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>456</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>458</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>462</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>472</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>474</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>476</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>478</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>482</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>488</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>494</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>498</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Etanol!$AE$3:$AE$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>16898.028844935237</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16865.027498427335</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16831.758161298741</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16798.224763606981</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16764.431241523485</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16730.353545831127</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16695.995966247374</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16661.335039454039</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16626.403060588276</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16591.149285502153</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16555.60614212988</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16519.751014312715</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16483.561768026833</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16447.07085891538</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16410.256410256414</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16373.070229010133</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16335.571851196008</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16297.713593759934</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16259.501646274541</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16220.915897795256</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16181.962936832089</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16142.62330542812</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>16102.903997706946</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16062.786218771937</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16022.277374461453</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>15981.359342462951</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15940.014537293257</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>15898.25119236884</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>15856.052413766862</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15813.401858074718</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15770.308609169171</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15726.732299562796</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15682.707462616347</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>15638.194726800737</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>15593.20448148697</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>15547.722958234152</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>15501.712939279791</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>15455.186142261899</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>15408.130562335135</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>15360.558387018484</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>15312.41147512116</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>15263.703371294163</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>15214.42449157197</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>15164.565868808308</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>15114.096313067346</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>15063.031254283551</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>15011.341068177007</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>14959.019765352816</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>14906.039778257751</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>14852.396879808461</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>14798.065596865179</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>14743.065230692115</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>14687.350372618079</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>14630.898995588783</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>14573.711647456084</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>14515.789550083104</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>14457.071893572818</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>14397.58350958375</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>14337.267001489643</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>14276.128884891574</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>14214.156162405263</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>14151.297178655881</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>14087.562654434907</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>14022.92467726239</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>13957.338000667161</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>13890.798873734027</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>13823.285877992916</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>13754.760866604953</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>13685.207385632722</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>13614.592665002056</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>13542.886937208405</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>13470.063457468948</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>13396.098520266958</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>13320.935982245855</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>13244.577007944097</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>13166.938344494509</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>13088.028772722455</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>13007.774746966261</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>12926.159314913557</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>12843.120004829012</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>12758.633448288621</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>12672.616882713664</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>12585.043430984881</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>12495.829516898733</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>12404.962481190976</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>12312.329320334797</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>12217.903871975916</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>12121.579441801267</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>12023.305976304468</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>11923.001257876633</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>11820.554525853917</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>11715.871373791362</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>11608.873823150416</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>11499.421004152442</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>11387.407576953252</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>11272.698988500719</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>11155.12427366197</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>11034.543638861456</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>10910.765215607631</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>10783.601162040861</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>10652.803817964888</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B2BE-479E-9001-C8AEBD48EE04}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="430249624"/>
+        <c:axId val="430254216"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="430249624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="430254216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="430254216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="430249624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
@@ -2948,6 +4193,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent3"/>
@@ -2985,6 +4270,522 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4829,6 +6630,36 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>392206</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>6723</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>280148</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>123264</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8500,23 +10331,381 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:Y51"/>
+  <dimension ref="B3:AE103"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA3">
+        <v>191</v>
+      </c>
+      <c r="AB3">
+        <v>881.84400000000005</v>
+      </c>
+      <c r="AC3">
+        <f>AB3/0.046</f>
+        <v>19170.521739130436</v>
+      </c>
+      <c r="AD3">
+        <v>300</v>
+      </c>
+      <c r="AE3">
+        <v>16898.028844935237</v>
+      </c>
+    </row>
+    <row r="4" spans="2:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AA4">
+        <v>197.44</v>
+      </c>
+      <c r="AB4">
+        <v>876.36900000000003</v>
+      </c>
+      <c r="AC4">
+        <f t="shared" ref="AC4:AC53" si="0">AB4/0.046</f>
+        <v>19051.5</v>
+      </c>
+      <c r="AD4">
+        <v>302</v>
+      </c>
+      <c r="AE4">
+        <v>16865.027498427335</v>
+      </c>
+    </row>
+    <row r="5" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA5">
+        <v>203.88</v>
+      </c>
+      <c r="AB5">
+        <v>870.85</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" si="0"/>
+        <v>18931.521739130436</v>
+      </c>
+      <c r="AD5">
+        <v>304</v>
+      </c>
+      <c r="AE5">
+        <v>16831.758161298741</v>
+      </c>
+    </row>
+    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA6">
+        <v>210.32</v>
+      </c>
+      <c r="AB6">
+        <v>865.28599999999994</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" si="0"/>
+        <v>18810.565217391304</v>
+      </c>
+      <c r="AD6">
+        <v>306</v>
+      </c>
+      <c r="AE6">
+        <v>16798.224763606981</v>
+      </c>
+    </row>
+    <row r="7" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA7">
+        <v>216.76</v>
+      </c>
+      <c r="AB7">
+        <v>859.67499999999995</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" si="0"/>
+        <v>18688.58695652174</v>
+      </c>
+      <c r="AD7">
+        <v>308</v>
+      </c>
+      <c r="AE7">
+        <v>16764.431241523485</v>
+      </c>
+    </row>
+    <row r="8" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA8">
+        <v>223.2</v>
+      </c>
+      <c r="AB8">
+        <v>854.01700000000005</v>
+      </c>
+      <c r="AC8">
+        <f t="shared" si="0"/>
+        <v>18565.58695652174</v>
+      </c>
+      <c r="AD8">
+        <v>310</v>
+      </c>
+      <c r="AE8">
+        <v>16730.353545831127</v>
+      </c>
+    </row>
+    <row r="9" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA9">
+        <v>229.64</v>
+      </c>
+      <c r="AB9">
+        <v>848.30799999999999</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="0"/>
+        <v>18441.478260869564</v>
+      </c>
+      <c r="AD9">
+        <v>312</v>
+      </c>
+      <c r="AE9">
+        <v>16695.995966247374</v>
+      </c>
+    </row>
+    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA10">
+        <v>236.08</v>
+      </c>
+      <c r="AB10">
+        <v>842.548</v>
+      </c>
+      <c r="AC10">
+        <f t="shared" si="0"/>
+        <v>18316.260869565216</v>
+      </c>
+      <c r="AD10">
+        <v>314</v>
+      </c>
+      <c r="AE10">
+        <v>16661.335039454039</v>
+      </c>
+    </row>
+    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA11">
+        <v>242.52</v>
+      </c>
+      <c r="AB11">
+        <v>836.73400000000004</v>
+      </c>
+      <c r="AC11">
+        <f t="shared" si="0"/>
+        <v>18189.869565217392</v>
+      </c>
+      <c r="AD11">
+        <v>316</v>
+      </c>
+      <c r="AE11">
+        <v>16626.403060588276</v>
+      </c>
+    </row>
+    <row r="12" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA12">
+        <v>248.96</v>
+      </c>
+      <c r="AB12">
+        <v>830.86400000000003</v>
+      </c>
+      <c r="AC12">
+        <f t="shared" si="0"/>
+        <v>18062.26086956522</v>
+      </c>
+      <c r="AD12">
+        <v>318</v>
+      </c>
+      <c r="AE12">
+        <v>16591.149285502153</v>
+      </c>
+    </row>
+    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA13">
+        <v>255.4</v>
+      </c>
+      <c r="AB13">
+        <v>824.93700000000001</v>
+      </c>
+      <c r="AC13">
+        <f t="shared" si="0"/>
+        <v>17933.41304347826</v>
+      </c>
+      <c r="AD13">
+        <v>320</v>
+      </c>
+      <c r="AE13">
+        <v>16555.60614212988</v>
+      </c>
+    </row>
+    <row r="14" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA14">
+        <v>261.83999999999997</v>
+      </c>
+      <c r="AB14">
+        <v>818.94799999999998</v>
+      </c>
+      <c r="AC14">
+        <f t="shared" si="0"/>
+        <v>17803.217391304348</v>
+      </c>
+      <c r="AD14">
+        <v>322</v>
+      </c>
+      <c r="AE14">
+        <v>16519.751014312715</v>
+      </c>
+    </row>
+    <row r="15" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA15">
+        <v>268.27999999999997</v>
+      </c>
+      <c r="AB15">
+        <v>812.89700000000005</v>
+      </c>
+      <c r="AC15">
+        <f t="shared" si="0"/>
+        <v>17671.67391304348</v>
+      </c>
+      <c r="AD15">
+        <v>324</v>
+      </c>
+      <c r="AE15">
+        <v>16483.561768026833</v>
+      </c>
+    </row>
+    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA16">
+        <v>274.72000000000003</v>
+      </c>
+      <c r="AB16">
+        <v>806.78099999999995</v>
+      </c>
+      <c r="AC16">
+        <f t="shared" si="0"/>
+        <v>17538.717391304348</v>
+      </c>
+      <c r="AD16">
+        <v>326</v>
+      </c>
+      <c r="AE16">
+        <v>16447.07085891538</v>
+      </c>
+    </row>
+    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA17">
+        <v>281.16000000000003</v>
+      </c>
+      <c r="AB17">
+        <v>800.59500000000003</v>
+      </c>
+      <c r="AC17">
+        <f t="shared" si="0"/>
+        <v>17404.239130434784</v>
+      </c>
+      <c r="AD17">
+        <v>328</v>
+      </c>
+      <c r="AE17">
+        <v>16410.256410256414</v>
+      </c>
+    </row>
+    <row r="18" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA18">
+        <v>287.60000000000002</v>
+      </c>
+      <c r="AB18">
+        <v>794.33799999999997</v>
+      </c>
+      <c r="AC18">
+        <f t="shared" si="0"/>
+        <v>17268.217391304348</v>
+      </c>
+      <c r="AD18">
+        <v>330</v>
+      </c>
+      <c r="AE18">
+        <v>16373.070229010133</v>
+      </c>
+    </row>
+    <row r="19" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA19">
+        <v>294.04000000000002</v>
+      </c>
+      <c r="AB19">
+        <v>788.00599999999997</v>
+      </c>
+      <c r="AC19">
+        <f t="shared" si="0"/>
+        <v>17130.565217391304</v>
+      </c>
+      <c r="AD19">
+        <v>332</v>
+      </c>
+      <c r="AE19">
+        <v>16335.571851196008</v>
+      </c>
+    </row>
+    <row r="20" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA20">
+        <v>300.48</v>
+      </c>
+      <c r="AB20">
+        <v>781.596</v>
+      </c>
+      <c r="AC20">
+        <f t="shared" si="0"/>
+        <v>16991.217391304348</v>
+      </c>
+      <c r="AD20">
+        <v>334</v>
+      </c>
+      <c r="AE20">
+        <v>16297.713593759934</v>
+      </c>
+    </row>
+    <row r="21" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA21">
+        <v>306.92</v>
+      </c>
+      <c r="AB21">
+        <v>775.10299999999995</v>
+      </c>
+      <c r="AC21">
+        <f t="shared" si="0"/>
+        <v>16850.065217391304</v>
+      </c>
+      <c r="AD21">
+        <v>336</v>
+      </c>
+      <c r="AE21">
+        <v>16259.501646274541</v>
+      </c>
+    </row>
+    <row r="22" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA22">
+        <v>313.36</v>
+      </c>
+      <c r="AB22">
+        <v>768.52300000000002</v>
+      </c>
+      <c r="AC22">
+        <f t="shared" si="0"/>
+        <v>16707.021739130436</v>
+      </c>
+      <c r="AD22">
+        <v>338</v>
+      </c>
+      <c r="AE22">
+        <v>16220.915897795256</v>
+      </c>
+    </row>
+    <row r="23" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
         <v>13</v>
       </c>
@@ -8544,8 +10733,24 @@
       <c r="W23" s="11"/>
       <c r="X23" s="11"/>
       <c r="Y23" s="11"/>
-    </row>
-    <row r="24" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA23">
+        <v>319.8</v>
+      </c>
+      <c r="AB23">
+        <v>761.85199999999998</v>
+      </c>
+      <c r="AC23">
+        <f t="shared" si="0"/>
+        <v>16562</v>
+      </c>
+      <c r="AD23">
+        <v>340</v>
+      </c>
+      <c r="AE23">
+        <v>16181.962936832089</v>
+      </c>
+    </row>
+    <row r="24" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -8567,8 +10772,24 @@
       <c r="W24" s="11"/>
       <c r="X24" s="11"/>
       <c r="Y24" s="11"/>
-    </row>
-    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AA24">
+        <v>326.24</v>
+      </c>
+      <c r="AB24">
+        <v>755.08399999999995</v>
+      </c>
+      <c r="AC24">
+        <f t="shared" si="0"/>
+        <v>16414.869565217392</v>
+      </c>
+      <c r="AD24">
+        <v>342</v>
+      </c>
+      <c r="AE24">
+        <v>16142.62330542812</v>
+      </c>
+    </row>
+    <row r="25" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
@@ -8590,8 +10811,24 @@
       <c r="W25" s="11"/>
       <c r="X25" s="11"/>
       <c r="Y25" s="11"/>
-    </row>
-    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AA25">
+        <v>332.68</v>
+      </c>
+      <c r="AB25">
+        <v>748.21500000000003</v>
+      </c>
+      <c r="AC25">
+        <f t="shared" si="0"/>
+        <v>16265.54347826087</v>
+      </c>
+      <c r="AD25">
+        <v>344</v>
+      </c>
+      <c r="AE25">
+        <v>16102.903997706946</v>
+      </c>
+    </row>
+    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -8613,8 +10850,24 @@
       <c r="W26" s="11"/>
       <c r="X26" s="11"/>
       <c r="Y26" s="11"/>
-    </row>
-    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="AA26">
+        <v>339.12</v>
+      </c>
+      <c r="AB26">
+        <v>741.23900000000003</v>
+      </c>
+      <c r="AC26">
+        <f t="shared" si="0"/>
+        <v>16113.891304347828</v>
+      </c>
+      <c r="AD26">
+        <v>346</v>
+      </c>
+      <c r="AE26">
+        <v>16062.786218771937</v>
+      </c>
+    </row>
+    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
       <c r="K27" s="11"/>
       <c r="L27" s="11"/>
       <c r="M27" s="11"/>
@@ -8629,13 +10882,387 @@
       <c r="W27" s="11"/>
       <c r="X27" s="11"/>
       <c r="Y27" s="11"/>
-    </row>
-    <row r="29" spans="2:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AA27">
+        <v>345.56</v>
+      </c>
+      <c r="AB27">
+        <v>734.14800000000002</v>
+      </c>
+      <c r="AC27">
+        <f t="shared" si="0"/>
+        <v>15959.739130434784</v>
+      </c>
+      <c r="AD27">
+        <v>348</v>
+      </c>
+      <c r="AE27">
+        <v>16022.277374461453</v>
+      </c>
+    </row>
+    <row r="28" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA28">
+        <v>352</v>
+      </c>
+      <c r="AB28">
+        <v>726.93600000000004</v>
+      </c>
+      <c r="AC28">
+        <f t="shared" si="0"/>
+        <v>15802.956521739132</v>
+      </c>
+      <c r="AD28">
+        <v>350</v>
+      </c>
+      <c r="AE28">
+        <v>15981.359342462951</v>
+      </c>
+    </row>
+    <row r="29" spans="2:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="AA29">
+        <v>358.44</v>
+      </c>
+      <c r="AB29">
+        <v>719.59400000000005</v>
+      </c>
+      <c r="AC29">
+        <f t="shared" si="0"/>
+        <v>15643.347826086958</v>
+      </c>
+      <c r="AD29">
+        <v>352</v>
+      </c>
+      <c r="AE29">
+        <v>15940.014537293257</v>
+      </c>
+    </row>
+    <row r="30" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA30">
+        <v>364.88</v>
+      </c>
+      <c r="AB30">
+        <v>712.11500000000001</v>
+      </c>
+      <c r="AC30">
+        <f t="shared" si="0"/>
+        <v>15480.760869565218</v>
+      </c>
+      <c r="AD30">
+        <v>354</v>
+      </c>
+      <c r="AE30">
+        <v>15898.25119236884</v>
+      </c>
+    </row>
+    <row r="31" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA31">
+        <v>371.32</v>
+      </c>
+      <c r="AB31">
+        <v>704.48800000000006</v>
+      </c>
+      <c r="AC31">
+        <f t="shared" si="0"/>
+        <v>15314.956521739132</v>
+      </c>
+      <c r="AD31">
+        <v>356</v>
+      </c>
+      <c r="AE31">
+        <v>15856.052413766862</v>
+      </c>
+    </row>
+    <row r="32" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA32">
+        <v>377.76</v>
+      </c>
+      <c r="AB32">
+        <v>696.702</v>
+      </c>
+      <c r="AC32">
+        <f t="shared" si="0"/>
+        <v>15145.695652173914</v>
+      </c>
+      <c r="AD32">
+        <v>358</v>
+      </c>
+      <c r="AE32">
+        <v>15813.401858074718</v>
+      </c>
+    </row>
+    <row r="33" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA33">
+        <v>384.2</v>
+      </c>
+      <c r="AB33">
+        <v>688.74400000000003</v>
+      </c>
+      <c r="AC33">
+        <f t="shared" si="0"/>
+        <v>14972.695652173914</v>
+      </c>
+      <c r="AD33">
+        <v>360</v>
+      </c>
+      <c r="AE33">
+        <v>15770.308609169171</v>
+      </c>
+    </row>
+    <row r="34" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA34">
+        <v>390.64</v>
+      </c>
+      <c r="AB34">
+        <v>680.601</v>
+      </c>
+      <c r="AC34">
+        <f t="shared" si="0"/>
+        <v>14795.673913043478</v>
+      </c>
+      <c r="AD34">
+        <v>362</v>
+      </c>
+      <c r="AE34">
+        <v>15726.732299562796</v>
+      </c>
+    </row>
+    <row r="35" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA35">
+        <v>397.08</v>
+      </c>
+      <c r="AB35">
+        <v>672.25699999999995</v>
+      </c>
+      <c r="AC35">
+        <f t="shared" si="0"/>
+        <v>14614.282608695652</v>
+      </c>
+      <c r="AD35">
+        <v>364</v>
+      </c>
+      <c r="AE35">
+        <v>15682.707462616347</v>
+      </c>
+    </row>
+    <row r="36" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA36">
+        <v>403.52</v>
+      </c>
+      <c r="AB36">
+        <v>663.69299999999998</v>
+      </c>
+      <c r="AC36">
+        <f t="shared" si="0"/>
+        <v>14428.108695652174</v>
+      </c>
+      <c r="AD36">
+        <v>366</v>
+      </c>
+      <c r="AE36">
+        <v>15638.194726800737</v>
+      </c>
+    </row>
+    <row r="37" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA37">
+        <v>409.96</v>
+      </c>
+      <c r="AB37">
+        <v>654.88800000000003</v>
+      </c>
+      <c r="AC37">
+        <f t="shared" si="0"/>
+        <v>14236.695652173914</v>
+      </c>
+      <c r="AD37">
+        <v>368</v>
+      </c>
+      <c r="AE37">
+        <v>15593.20448148697</v>
+      </c>
+    </row>
+    <row r="38" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA38">
+        <v>416.4</v>
+      </c>
+      <c r="AB38">
+        <v>645.81799999999998</v>
+      </c>
+      <c r="AC38">
+        <f t="shared" si="0"/>
+        <v>14039.521739130434</v>
+      </c>
+      <c r="AD38">
+        <v>370</v>
+      </c>
+      <c r="AE38">
+        <v>15547.722958234152</v>
+      </c>
+    </row>
+    <row r="39" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA39">
+        <v>422.84</v>
+      </c>
+      <c r="AB39">
+        <v>636.452</v>
+      </c>
+      <c r="AC39">
+        <f t="shared" si="0"/>
+        <v>13835.913043478262</v>
+      </c>
+      <c r="AD39">
+        <v>372</v>
+      </c>
+      <c r="AE39">
+        <v>15501.712939279791</v>
+      </c>
+    </row>
+    <row r="40" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA40">
+        <v>429.28</v>
+      </c>
+      <c r="AB40">
+        <v>626.75599999999997</v>
+      </c>
+      <c r="AC40">
+        <f t="shared" si="0"/>
+        <v>13625.130434782608</v>
+      </c>
+      <c r="AD40">
+        <v>374</v>
+      </c>
+      <c r="AE40">
+        <v>15455.186142261899</v>
+      </c>
+    </row>
+    <row r="41" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA41">
+        <v>435.72</v>
+      </c>
+      <c r="AB41">
+        <v>616.68899999999996</v>
+      </c>
+      <c r="AC41">
+        <f t="shared" si="0"/>
+        <v>13406.282608695652</v>
+      </c>
+      <c r="AD41">
+        <v>376</v>
+      </c>
+      <c r="AE41">
+        <v>15408.130562335135</v>
+      </c>
+    </row>
+    <row r="42" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA42">
+        <v>442.16</v>
+      </c>
+      <c r="AB42">
+        <v>606.19799999999998</v>
+      </c>
+      <c r="AC42">
+        <f t="shared" si="0"/>
+        <v>13178.217391304348</v>
+      </c>
+      <c r="AD42">
+        <v>378</v>
+      </c>
+      <c r="AE42">
+        <v>15360.558387018484</v>
+      </c>
+    </row>
+    <row r="43" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA43">
+        <v>448.6</v>
+      </c>
+      <c r="AB43">
+        <v>595.22</v>
+      </c>
+      <c r="AC43">
+        <f t="shared" si="0"/>
+        <v>12939.565217391306</v>
+      </c>
+      <c r="AD43">
+        <v>380</v>
+      </c>
+      <c r="AE43">
+        <v>15312.41147512116</v>
+      </c>
+    </row>
+    <row r="44" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA44">
+        <v>455.04</v>
+      </c>
+      <c r="AB44">
+        <v>583.67399999999998</v>
+      </c>
+      <c r="AC44">
+        <f t="shared" si="0"/>
+        <v>12688.565217391304</v>
+      </c>
+      <c r="AD44">
+        <v>382</v>
+      </c>
+      <c r="AE44">
+        <v>15263.703371294163</v>
+      </c>
+    </row>
+    <row r="45" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA45">
+        <v>461.48</v>
+      </c>
+      <c r="AB45">
+        <v>571.452</v>
+      </c>
+      <c r="AC45">
+        <f t="shared" si="0"/>
+        <v>12422.869565217392</v>
+      </c>
+      <c r="AD45">
+        <v>384</v>
+      </c>
+      <c r="AE45">
+        <v>15214.42449157197</v>
+      </c>
+    </row>
+    <row r="46" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA46">
+        <v>467.92</v>
+      </c>
+      <c r="AB46">
+        <v>558.41300000000001</v>
+      </c>
+      <c r="AC46">
+        <f t="shared" si="0"/>
+        <v>12139.413043478262</v>
+      </c>
+      <c r="AD46">
+        <v>386</v>
+      </c>
+      <c r="AE46">
+        <v>15164.565868808308</v>
+      </c>
+    </row>
+    <row r="47" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA47">
+        <v>474.36</v>
+      </c>
+      <c r="AB47">
+        <v>544.35699999999997</v>
+      </c>
+      <c r="AC47">
+        <f t="shared" si="0"/>
+        <v>11833.847826086956</v>
+      </c>
+      <c r="AD47">
+        <v>388</v>
+      </c>
+      <c r="AE47">
+        <v>15114.096313067346</v>
+      </c>
+    </row>
+    <row r="48" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B48" s="12" t="s">
         <v>130</v>
       </c>
@@ -8645,8 +11272,24 @@
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
       <c r="H48" s="12"/>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="AA48">
+        <v>480.8</v>
+      </c>
+      <c r="AB48">
+        <v>528.99400000000003</v>
+      </c>
+      <c r="AC48">
+        <f t="shared" si="0"/>
+        <v>11499.869565217392</v>
+      </c>
+      <c r="AD48">
+        <v>390</v>
+      </c>
+      <c r="AE48">
+        <v>15063.031254283551</v>
+      </c>
+    </row>
+    <row r="49" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
@@ -8654,8 +11297,24 @@
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="AA49">
+        <v>487.24</v>
+      </c>
+      <c r="AB49">
+        <v>511.86799999999999</v>
+      </c>
+      <c r="AC49">
+        <f t="shared" si="0"/>
+        <v>11127.565217391304</v>
+      </c>
+      <c r="AD49">
+        <v>392</v>
+      </c>
+      <c r="AE49">
+        <v>15011.341068177007</v>
+      </c>
+    </row>
+    <row r="50" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
@@ -8663,8 +11322,24 @@
       <c r="F50" s="12"/>
       <c r="G50" s="12"/>
       <c r="H50" s="12"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="AA50">
+        <v>493.68</v>
+      </c>
+      <c r="AB50">
+        <v>492.18799999999999</v>
+      </c>
+      <c r="AC50">
+        <f t="shared" si="0"/>
+        <v>10699.739130434782</v>
+      </c>
+      <c r="AD50">
+        <v>394</v>
+      </c>
+      <c r="AE50">
+        <v>14959.019765352816</v>
+      </c>
+    </row>
+    <row r="51" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
@@ -8672,6 +11347,458 @@
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
       <c r="H51" s="12"/>
+      <c r="AA51">
+        <v>500.12</v>
+      </c>
+      <c r="AB51">
+        <v>468.36599999999999</v>
+      </c>
+      <c r="AC51">
+        <f t="shared" si="0"/>
+        <v>10181.869565217392</v>
+      </c>
+      <c r="AD51">
+        <v>396</v>
+      </c>
+      <c r="AE51">
+        <v>14906.039778257751</v>
+      </c>
+    </row>
+    <row r="52" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA52">
+        <v>506.56</v>
+      </c>
+      <c r="AB52">
+        <v>436.09199999999998</v>
+      </c>
+      <c r="AC52">
+        <f t="shared" si="0"/>
+        <v>9480.2608695652179</v>
+      </c>
+      <c r="AD52">
+        <v>398</v>
+      </c>
+      <c r="AE52">
+        <v>14852.396879808461</v>
+      </c>
+    </row>
+    <row r="53" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AA53">
+        <v>513</v>
+      </c>
+      <c r="AB53">
+        <v>354.64400000000001</v>
+      </c>
+      <c r="AC53">
+        <f t="shared" si="0"/>
+        <v>7709.652173913044</v>
+      </c>
+      <c r="AD53">
+        <v>400</v>
+      </c>
+      <c r="AE53">
+        <v>14798.065596865179</v>
+      </c>
+    </row>
+    <row r="54" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AD54">
+        <v>402</v>
+      </c>
+      <c r="AE54">
+        <v>14743.065230692115</v>
+      </c>
+    </row>
+    <row r="55" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AD55">
+        <v>404</v>
+      </c>
+      <c r="AE55">
+        <v>14687.350372618079</v>
+      </c>
+    </row>
+    <row r="56" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AD56">
+        <v>406</v>
+      </c>
+      <c r="AE56">
+        <v>14630.898995588783</v>
+      </c>
+    </row>
+    <row r="57" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AD57">
+        <v>408</v>
+      </c>
+      <c r="AE57">
+        <v>14573.711647456084</v>
+      </c>
+    </row>
+    <row r="58" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AD58">
+        <v>410</v>
+      </c>
+      <c r="AE58">
+        <v>14515.789550083104</v>
+      </c>
+    </row>
+    <row r="59" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AD59">
+        <v>412</v>
+      </c>
+      <c r="AE59">
+        <v>14457.071893572818</v>
+      </c>
+    </row>
+    <row r="60" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AD60">
+        <v>414</v>
+      </c>
+      <c r="AE60">
+        <v>14397.58350958375</v>
+      </c>
+    </row>
+    <row r="61" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AD61">
+        <v>416</v>
+      </c>
+      <c r="AE61">
+        <v>14337.267001489643</v>
+      </c>
+    </row>
+    <row r="62" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AD62">
+        <v>418</v>
+      </c>
+      <c r="AE62">
+        <v>14276.128884891574</v>
+      </c>
+    </row>
+    <row r="63" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AD63">
+        <v>420</v>
+      </c>
+      <c r="AE63">
+        <v>14214.156162405263</v>
+      </c>
+    </row>
+    <row r="64" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="AD64">
+        <v>422</v>
+      </c>
+      <c r="AE64">
+        <v>14151.297178655881</v>
+      </c>
+    </row>
+    <row r="65" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD65">
+        <v>424</v>
+      </c>
+      <c r="AE65">
+        <v>14087.562654434907</v>
+      </c>
+    </row>
+    <row r="66" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD66">
+        <v>426</v>
+      </c>
+      <c r="AE66">
+        <v>14022.92467726239</v>
+      </c>
+    </row>
+    <row r="67" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD67">
+        <v>428</v>
+      </c>
+      <c r="AE67">
+        <v>13957.338000667161</v>
+      </c>
+    </row>
+    <row r="68" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD68">
+        <v>430</v>
+      </c>
+      <c r="AE68">
+        <v>13890.798873734027</v>
+      </c>
+    </row>
+    <row r="69" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD69">
+        <v>432</v>
+      </c>
+      <c r="AE69">
+        <v>13823.285877992916</v>
+      </c>
+    </row>
+    <row r="70" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD70">
+        <v>434</v>
+      </c>
+      <c r="AE70">
+        <v>13754.760866604953</v>
+      </c>
+    </row>
+    <row r="71" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD71">
+        <v>436</v>
+      </c>
+      <c r="AE71">
+        <v>13685.207385632722</v>
+      </c>
+    </row>
+    <row r="72" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD72">
+        <v>438</v>
+      </c>
+      <c r="AE72">
+        <v>13614.592665002056</v>
+      </c>
+    </row>
+    <row r="73" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD73">
+        <v>440</v>
+      </c>
+      <c r="AE73">
+        <v>13542.886937208405</v>
+      </c>
+    </row>
+    <row r="74" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD74">
+        <v>442</v>
+      </c>
+      <c r="AE74">
+        <v>13470.063457468948</v>
+      </c>
+    </row>
+    <row r="75" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD75">
+        <v>444</v>
+      </c>
+      <c r="AE75">
+        <v>13396.098520266958</v>
+      </c>
+    </row>
+    <row r="76" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD76">
+        <v>446</v>
+      </c>
+      <c r="AE76">
+        <v>13320.935982245855</v>
+      </c>
+    </row>
+    <row r="77" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD77">
+        <v>448</v>
+      </c>
+      <c r="AE77">
+        <v>13244.577007944097</v>
+      </c>
+    </row>
+    <row r="78" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD78">
+        <v>450</v>
+      </c>
+      <c r="AE78">
+        <v>13166.938344494509</v>
+      </c>
+    </row>
+    <row r="79" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD79">
+        <v>452</v>
+      </c>
+      <c r="AE79">
+        <v>13088.028772722455</v>
+      </c>
+    </row>
+    <row r="80" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD80">
+        <v>454</v>
+      </c>
+      <c r="AE80">
+        <v>13007.774746966261</v>
+      </c>
+    </row>
+    <row r="81" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD81">
+        <v>456</v>
+      </c>
+      <c r="AE81">
+        <v>12926.159314913557</v>
+      </c>
+    </row>
+    <row r="82" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD82">
+        <v>458</v>
+      </c>
+      <c r="AE82">
+        <v>12843.120004829012</v>
+      </c>
+    </row>
+    <row r="83" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD83">
+        <v>460</v>
+      </c>
+      <c r="AE83">
+        <v>12758.633448288621</v>
+      </c>
+    </row>
+    <row r="84" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD84">
+        <v>462</v>
+      </c>
+      <c r="AE84">
+        <v>12672.616882713664</v>
+      </c>
+    </row>
+    <row r="85" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD85">
+        <v>464</v>
+      </c>
+      <c r="AE85">
+        <v>12585.043430984881</v>
+      </c>
+    </row>
+    <row r="86" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD86">
+        <v>466</v>
+      </c>
+      <c r="AE86">
+        <v>12495.829516898733</v>
+      </c>
+    </row>
+    <row r="87" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD87">
+        <v>468</v>
+      </c>
+      <c r="AE87">
+        <v>12404.962481190976</v>
+      </c>
+    </row>
+    <row r="88" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD88">
+        <v>470</v>
+      </c>
+      <c r="AE88">
+        <v>12312.329320334797</v>
+      </c>
+    </row>
+    <row r="89" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD89">
+        <v>472</v>
+      </c>
+      <c r="AE89">
+        <v>12217.903871975916</v>
+      </c>
+    </row>
+    <row r="90" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD90">
+        <v>474</v>
+      </c>
+      <c r="AE90">
+        <v>12121.579441801267</v>
+      </c>
+    </row>
+    <row r="91" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD91">
+        <v>476</v>
+      </c>
+      <c r="AE91">
+        <v>12023.305976304468</v>
+      </c>
+    </row>
+    <row r="92" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD92">
+        <v>478</v>
+      </c>
+      <c r="AE92">
+        <v>11923.001257876633</v>
+      </c>
+    </row>
+    <row r="93" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD93">
+        <v>480</v>
+      </c>
+      <c r="AE93">
+        <v>11820.554525853917</v>
+      </c>
+    </row>
+    <row r="94" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD94">
+        <v>482</v>
+      </c>
+      <c r="AE94">
+        <v>11715.871373791362</v>
+      </c>
+    </row>
+    <row r="95" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD95">
+        <v>484</v>
+      </c>
+      <c r="AE95">
+        <v>11608.873823150416</v>
+      </c>
+    </row>
+    <row r="96" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD96">
+        <v>486</v>
+      </c>
+      <c r="AE96">
+        <v>11499.421004152442</v>
+      </c>
+    </row>
+    <row r="97" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD97">
+        <v>488</v>
+      </c>
+      <c r="AE97">
+        <v>11387.407576953252</v>
+      </c>
+    </row>
+    <row r="98" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD98">
+        <v>490</v>
+      </c>
+      <c r="AE98">
+        <v>11272.698988500719</v>
+      </c>
+    </row>
+    <row r="99" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD99">
+        <v>492</v>
+      </c>
+      <c r="AE99">
+        <v>11155.12427366197</v>
+      </c>
+    </row>
+    <row r="100" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD100">
+        <v>494</v>
+      </c>
+      <c r="AE100">
+        <v>11034.543638861456</v>
+      </c>
+    </row>
+    <row r="101" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD101">
+        <v>496</v>
+      </c>
+      <c r="AE101">
+        <v>10910.765215607631</v>
+      </c>
+    </row>
+    <row r="102" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD102">
+        <v>498</v>
+      </c>
+      <c r="AE102">
+        <v>10783.601162040861</v>
+      </c>
+    </row>
+    <row r="103" spans="30:31" x14ac:dyDescent="0.25">
+      <c r="AD103">
+        <v>500</v>
+      </c>
+      <c r="AE103">
+        <v>10652.803817964888</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -8681,7 +11808,8 @@
     <mergeCell ref="B48:H51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8689,7 +11817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>

</xml_diff>